<commit_message>
wartości domyślne dla PSO
</commit_message>
<xml_diff>
--- a/a1/1.xlsx
+++ b/a1/1.xlsx
@@ -337,10 +337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -357,17 +357,27 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>